<commit_message>
Refactored instance loading to use monthly filters; started add-transaction feature
- Modified instance loading to only pull transactions by selected month and year,
  rather than the full Excel dataset, to reduce memory usage.
- Began implementing the "Add Transaction" button and pop-up UI.
  Currently incomplete — input handling and data persistence still needed.
</commit_message>
<xml_diff>
--- a/master_transaction.xlsx
+++ b/master_transaction.xlsx
@@ -65,12 +65,26 @@
       <number:text>/</number:text>
       <number:year/>
     </number:date-style>
-    <style:style style:name="ce1" style:family="table-cell" style:parent-style-name="Default">
+    <number:date-style style:name="N37" number:automatic-order="true">
+      <number:month number:style="long"/>
+      <number:text>/</number:text>
+      <number:day number:style="long"/>
+      <number:text>/</number:text>
+      <number:year/>
+    </number:date-style>
+    <number:time-style style:name="N61">
+      <number:hours number:style="long"/>
+      <number:text>:</number:text>
+      <number:minutes number:style="long"/>
+      <number:text>:</number:text>
+      <number:seconds number:style="long"/>
+    </number:time-style>
+    <style:style style:name="ce2" style:family="table-cell" style:parent-style-name="Default">
       <style:table-cell-properties style:diagonal-bl-tr="none" style:diagonal-tl-br="none" style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="no-wrap" fo:border="0.74pt solid #000000" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="top" loext:vertical-justify="auto"/>
       <style:paragraph-properties fo:text-align="center" css3t:text-justify="auto" fo:margin-left="0in" style:writing-mode="page"/>
       <style:text-properties fo:color="#000000" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Calibri" fo:font-size="11pt" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="bold" style:font-size-asian="11pt" style:font-style-asian="normal" style:font-weight-asian="bold" style:font-name-complex="Calibri" style:font-size-complex="11pt" style:font-style-complex="normal" style:font-weight-complex="bold"/>
     </style:style>
-    <style:style style:name="ce4" style:family="table-cell" style:parent-style-name="Default">
+    <style:style style:name="ce3" style:family="table-cell" style:parent-style-name="Default">
       <style:table-cell-properties style:diagonal-bl-tr="none" style:diagonal-tl-br="none" style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="no-wrap" fo:border="0.74pt solid #000000" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="top" loext:vertical-justify="auto"/>
       <style:paragraph-properties fo:text-align="center" css3t:text-justify="auto" fo:margin-left="0in" style:writing-mode="page"/>
       <style:text-properties fo:color="#000000" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Calibri" fo:font-size="11pt" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="bold" style:font-size-asian="11pt" style:font-style-asian="normal" style:font-weight-asian="bold" style:font-name-complex="Calibri" style:font-size-complex="11pt" style:font-style-complex="normal" style:font-weight-complex="bold"/>
@@ -78,6 +92,8 @@
     <style:style style:name="ce5" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N30">
       <style:table-cell-properties style:rotation-align="none"/>
     </style:style>
+    <style:style style:name="ce6" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N37"/>
+    <style:style style:name="ce7" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N61"/>
   </office:automatic-styles>
   <office:body>
     <office:spreadsheet>
@@ -92,16 +108,16 @@
         <table:table-column table:style-name="co4" table:default-cell-style-name="Default"/>
         <table:table-column table:style-name="co5" table:number-columns-repeated="1020" table:default-cell-style-name="Default"/>
         <table:table-row table:style-name="ro1">
-          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce3" office:value-type="string" calcext:value-type="string">
             <text:p>Starting Balance</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce3" office:value-type="string" calcext:value-type="string">
             <text:p>Total Credits</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce3" office:value-type="string" calcext:value-type="string">
             <text:p>Total Debits</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce3" office:value-type="string" calcext:value-type="string">
             <text:p>Ending Balance</text:p>
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1020"/>
@@ -137,19 +153,19 @@
         <table:table-column table:style-name="co9" table:default-cell-style-name="Default"/>
         <table:table-column table:style-name="co5" table:number-columns-repeated="1019" table:default-cell-style-name="Default"/>
         <table:table-row table:style-name="ro1">
-          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce3" office:value-type="string" calcext:value-type="string">
             <text:p>Date</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce3" office:value-type="string" calcext:value-type="string">
             <text:p>Time</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce3" office:value-type="string" calcext:value-type="string">
             <text:p>Description</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce3" office:value-type="string" calcext:value-type="string">
             <text:p>Amount</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce3" office:value-type="string" calcext:value-type="string">
             <text:p>Balance</text:p>
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1019"/>
@@ -514,7 +530,25 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1019"/>
         </table:table-row>
-        <table:table-row table:style-name="ro1" table:number-rows-repeated="1048554">
+        <table:table-row table:style-name="ro1">
+          <table:table-cell table:style-name="ce6" office:value-type="date" office:date-value="2025-06-05" calcext:value-type="date">
+            <text:p>06/05/25</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce7" office:value-type="time" office:time-value="PT12H25M00S" calcext:value-type="time">
+            <text:p>12:25:00</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Test 21</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="-84.54" calcext:value-type="float">
+            <text:p>-84.54</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="1322.84" calcext:value-type="float">
+            <text:p>1322.84</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1019"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1" table:number-rows-repeated="1048553">
           <table:table-cell table:number-columns-repeated="1024"/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
@@ -531,11 +565,11 @@
 <office:document-meta xmlns:grddl="http://www.w3.org/2003/g/data-view#" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:ooo="http://openoffice.org/2004/office" xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" office:version="1.3">
   <office:meta>
     <meta:creation-date>2025-05-26T13:39:43</meta:creation-date>
-    <dc:date>2025-06-04T07:15:49.071878956</dc:date>
+    <dc:date>2025-06-08T12:55:16.964991491</dc:date>
     <meta:generator>LibreOffice/7.3.7.2$Linux_X86_64 LibreOffice_project/30$Build-2</meta:generator>
-    <meta:editing-duration>PT21M15S</meta:editing-duration>
-    <meta:editing-cycles>2</meta:editing-cycles>
-    <meta:document-statistic meta:table-count="2" meta:cell-count="113" meta:object-count="0"/>
+    <meta:editing-duration>PT31M7S</meta:editing-duration>
+    <meta:editing-cycles>4</meta:editing-cycles>
+    <meta:document-statistic meta:table-count="2" meta:cell-count="118" meta:object-count="0"/>
     <meta:user-defined meta:name="AppVersion">12.0000</meta:user-defined>
   </office:meta>
 </office:document-meta>
@@ -548,7 +582,7 @@
       <config:config-item config:name="VisibleAreaTop" config:type="int">0</config:config-item>
       <config:config-item config:name="VisibleAreaLeft" config:type="int">0</config:config-item>
       <config:config-item config:name="VisibleAreaWidth" config:type="int">21839</config:config-item>
-      <config:config-item config:name="VisibleAreaHeight" config:type="int">10224</config:config-item>
+      <config:config-item config:name="VisibleAreaHeight" config:type="int">10710</config:config-item>
       <config:config-item-map-indexed config:name="Views">
         <config:config-item-map-entry>
           <config:config-item config:name="ViewId" config:type="string">view1</config:config-item>
@@ -568,10 +602,10 @@
               <config:config-item config:name="AnchoredTextOverflowLegacy" config:type="boolean">false</config:config-item>
             </config:config-item-map-entry>
             <config:config-item-map-entry config:name="Transactions">
-              <config:config-item config:name="CursorPositionX" config:type="int">1</config:config-item>
-              <config:config-item config:name="CursorPositionY" config:type="int">26</config:config-item>
+              <config:config-item config:name="CursorPositionX" config:type="int">4</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">22</config:config-item>
               <config:config-item config:name="ActiveSplitRange" config:type="short">2</config:config-item>
-              <config:config-item config:name="PositionLeft" config:type="int">0</config:config-item>
+              <config:config-item config:name="PositionLeft" config:type="int">1</config:config-item>
               <config:config-item config:name="PositionRight" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionTop" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionBottom" config:type="int">0</config:config-item>
@@ -630,7 +664,7 @@
       <config:config-item config:name="LoadReadonly" config:type="boolean">false</config:config-item>
       <config:config-item config:name="PrinterName" config:type="string">Generic Printer</config:config-item>
       <config:config-item config:name="PrinterPaperFromSetup" config:type="boolean">false</config:config-item>
-      <config:config-item config:name="PrinterSetup" config:type="base64Binary">mAH+/0dlbmVyaWMgUHJpbnRlcgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAU0dFTlBSVAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAWAAMAuQAAAAAAAAAIAFZUAAAkbQAASm9iRGF0YSAxCnByaW50ZXI9R2VuZXJpYyBQcmludGVyCm9yaWVudGF0aW9uPVBvcnRyYWl0CmNvcGllcz0xCmNvbGxhdGU9ZmFsc2UKbWFyZ2luYWRqdXN0bWVudD0wLDAsMCwwCmNvbG9yZGVwdGg9MjQKcHNsZXZlbD0wCnBkZmRldmljZT0xCmNvbG9yZGV2aWNlPTAKUFBEQ29udGV4dERhdGEKUGFnZVNpemU6TGV0dGVyAAASAENPTVBBVF9EVVBMRVhfTU9ERQ8ARHVwbGV4TW9kZTo6T2Zm</config:config-item>
+      <config:config-item config:name="PrinterSetup" config:type="base64Binary">pAH+/0dlbmVyaWMgUHJpbnRlcgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAU0dFTlBSVAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAWAAMAxQAAAAAAAAAIAFZUAAAkbQAASm9iRGF0YSAxCnByaW50ZXI9R2VuZXJpYyBQcmludGVyCm9yaWVudGF0aW9uPVBvcnRyYWl0CmNvcGllcz0xCmNvbGxhdGU9ZmFsc2UKbWFyZ2luYWRqdXN0bWVudD0wLDAsMCwwCmNvbG9yZGVwdGg9MjQKcHNsZXZlbD0wCnBkZmRldmljZT0xCmNvbG9yZGV2aWNlPTAKUFBEQ29udGV4dERhdGEKUGFnZVNpemU6TGV0dGVyAER1cGxleDpOb25lAAASAENPTVBBVF9EVVBMRVhfTU9ERQ8ARHVwbGV4TW9kZTo6T2Zm</config:config-item>
       <config:config-item config:name="RasterIsVisible" config:type="boolean">false</config:config-item>
       <config:config-item config:name="RasterResolutionX" config:type="int">1270</config:config-item>
       <config:config-item config:name="RasterResolutionY" config:type="int">1270</config:config-item>
@@ -684,258 +718,258 @@
       <number:text>:</number:text>
       <number:minutes number:style="long"/>
     </number:date-style>
-    <number:time-style style:name="N158">
+    <number:number-style style:name="N157P0" style:volatile="true">
+      <number:text> </number:text>
+      <number:fill-character> </number:fill-character>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:number-style>
+    <number:number-style style:name="N157P1" style:volatile="true">
+      <number:text> </number:text>
+      <number:fill-character> </number:fill-character>
+      <number:text>(</number:text>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text>)</number:text>
+    </number:number-style>
+    <number:number-style style:name="N157P2" style:volatile="true">
+      <number:text> </number:text>
+      <number:fill-character> </number:fill-character>
+      <number:text>-</number:text>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="0"/>
+      <number:text> </number:text>
+    </number:number-style>
+    <number:text-style style:name="N157">
+      <number:text> </number:text>
+      <number:text-content/>
+      <number:text> </number:text>
+      <style:map style:condition="value()&gt;0" style:apply-style-name="N157P0"/>
+      <style:map style:condition="value()&lt;0" style:apply-style-name="N157P1"/>
+      <style:map style:condition="value()=0" style:apply-style-name="N157P2"/>
+    </number:text-style>
+    <number:time-style style:name="N153">
       <number:hours/>
       <number:text>:</number:text>
+      <number:minutes number:style="long"/>
+    </number:time-style>
+    <number:time-style style:name="N152">
+      <number:hours/>
+      <number:text>:</number:text>
+      <number:minutes number:style="long"/>
+      <number:text>:</number:text>
+      <number:seconds number:style="long"/>
+      <number:text> </number:text>
+      <number:am-pm/>
+    </number:time-style>
+    <number:time-style style:name="N151">
+      <number:hours/>
+      <number:text>:</number:text>
+      <number:minutes number:style="long"/>
+      <number:text> </number:text>
+      <number:am-pm/>
+    </number:time-style>
+    <number:currency-style style:name="N149P0" style:volatile="true">
+      <number:currency-symbol/>
+      <number:fill-character> </number:fill-character>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:currency-style>
+    <number:currency-style style:name="N149P1" style:volatile="true">
+      <number:currency-symbol/>
+      <number:fill-character> </number:fill-character>
+      <number:text>(</number:text>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text>)</number:text>
+    </number:currency-style>
+    <number:currency-style style:name="N149P2" style:volatile="true">
+      <number:currency-symbol/>
+      <number:fill-character> </number:fill-character>
+      <number:text>-</number:text>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="0"/>
+      <number:text> </number:text>
+    </number:currency-style>
+    <number:text-style style:name="N149">
+      <number:text> </number:text>
+      <number:text-content/>
+      <number:text> </number:text>
+      <style:map style:condition="value()&gt;0" style:apply-style-name="N149P0"/>
+      <style:map style:condition="value()&lt;0" style:apply-style-name="N149P1"/>
+      <style:map style:condition="value()=0" style:apply-style-name="N149P2"/>
+    </number:text-style>
+    <number:date-style style:name="N145">
+      <number:day/>
+      <number:text>-</number:text>
+      <number:month number:textual="true"/>
+    </number:date-style>
+    <number:time-style style:name="N144">
       <number:minutes number:style="long"/>
       <number:text>:</number:text>
       <number:seconds number:style="long"/>
     </number:time-style>
-    <number:time-style style:name="N157">
-      <number:hours/>
-      <number:text>:</number:text>
-      <number:minutes number:style="long"/>
-    </number:time-style>
-    <number:time-style style:name="N156">
-      <number:hours/>
-      <number:text>:</number:text>
-      <number:minutes number:style="long"/>
-      <number:text>:</number:text>
-      <number:seconds number:style="long"/>
-      <number:text> </number:text>
-      <number:am-pm/>
-    </number:time-style>
-    <number:time-style style:name="N155">
-      <number:hours/>
-      <number:text>:</number:text>
-      <number:minutes number:style="long"/>
-      <number:text> </number:text>
-      <number:am-pm/>
-    </number:time-style>
-    <number:date-style style:name="N154">
+    <number:date-style style:name="N150">
       <number:month number:textual="true"/>
       <number:text>-</number:text>
       <number:year/>
     </number:date-style>
-    <number:date-style style:name="N153">
+    <number:number-style style:name="N121">
+      <number:scientific-number number:decimal-places="1" number:min-decimal-places="1" number:min-integer-digits="1" number:min-exponent-digits="1" number:exponent-interval="3" number:forced-exponent-sign="true"/>
+    </number:number-style>
+    <number:currency-style style:name="N125P0" style:volatile="true">
+      <number:currency-symbol/>
+      <number:fill-character> </number:fill-character>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:currency-style>
+    <number:currency-style style:name="N125P1" style:volatile="true">
+      <number:currency-symbol/>
+      <number:fill-character> </number:fill-character>
+      <number:text>(</number:text>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text>)</number:text>
+    </number:currency-style>
+    <number:currency-style style:name="N125P2" style:volatile="true">
+      <number:currency-symbol/>
+      <number:fill-character> </number:fill-character>
+      <number:text>- </number:text>
+    </number:currency-style>
+    <number:text-style style:name="N125">
+      <number:text> </number:text>
+      <number:text-content/>
+      <number:text> </number:text>
+      <style:map style:condition="value()&gt;0" style:apply-style-name="N125P0"/>
+      <style:map style:condition="value()&lt;0" style:apply-style-name="N125P1"/>
+      <style:map style:condition="value()=0" style:apply-style-name="N125P2"/>
+    </number:text-style>
+    <number:currency-style style:name="N138P0" style:volatile="true">
+      <number:currency-symbol/>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:currency-style>
+    <number:currency-style style:name="N138">
+      <number:text>(</number:text>
+      <number:currency-symbol/>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text>)</number:text>
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N138P0"/>
+    </number:currency-style>
+    <number:time-style style:name="N158">
+      <number:hours/>
+      <number:text>:</number:text>
+      <number:minutes number:style="long"/>
+      <number:text>:</number:text>
+      <number:seconds number:style="long"/>
+    </number:time-style>
+    <number:number-style style:name="N129P0" style:volatile="true">
+      <number:text> </number:text>
+      <number:fill-character> </number:fill-character>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:number-style>
+    <number:number-style style:name="N129P1" style:volatile="true">
+      <number:text> </number:text>
+      <number:fill-character> </number:fill-character>
+      <number:text>(</number:text>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text>)</number:text>
+    </number:number-style>
+    <number:number-style style:name="N129P2" style:volatile="true">
+      <number:text> </number:text>
+      <number:fill-character> </number:fill-character>
+      <number:text>- </number:text>
+    </number:number-style>
+    <number:text-style style:name="N129">
+      <number:text> </number:text>
+      <number:text-content/>
+      <number:text> </number:text>
+      <style:map style:condition="value()&gt;0" style:apply-style-name="N129P0"/>
+      <style:map style:condition="value()&lt;0" style:apply-style-name="N129P1"/>
+      <style:map style:condition="value()=0" style:apply-style-name="N129P2"/>
+    </number:text-style>
+    <number:time-style style:name="N142" number:truncate-on-overflow="false">
+      <number:hours/>
+      <number:text>:</number:text>
+      <number:minutes number:style="long"/>
+      <number:text>:</number:text>
+      <number:seconds number:style="long"/>
+    </number:time-style>
+    <number:number-style style:name="N131P0" style:volatile="true">
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:number-style>
+    <number:number-style style:name="N131">
+      <style:text-properties fo:color="#ff0000"/>
+      <number:text>(</number:text>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text>)</number:text>
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N131P0"/>
+    </number:number-style>
+    <number:number-style style:name="N133P0" style:volatile="true">
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:number-style>
+    <number:number-style style:name="N133">
+      <style:text-properties fo:color="#ff0000"/>
+      <number:text>(</number:text>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text>)</number:text>
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N133P0"/>
+    </number:number-style>
+    <number:currency-style style:name="N135P0" style:volatile="true">
+      <number:currency-symbol/>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:currency-style>
+    <number:currency-style style:name="N135">
+      <number:text>(</number:text>
+      <number:currency-symbol/>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text>)</number:text>
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N135P0"/>
+    </number:currency-style>
+    <number:currency-style style:name="N136P0" style:volatile="true">
+      <number:currency-symbol/>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:currency-style>
+    <number:currency-style style:name="N136">
+      <style:text-properties fo:color="#ff0000"/>
+      <number:text>(</number:text>
+      <number:currency-symbol/>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text>)</number:text>
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N136P0"/>
+    </number:currency-style>
+    <number:currency-style style:name="N139P0" style:volatile="true">
+      <number:currency-symbol/>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:currency-style>
+    <number:currency-style style:name="N139">
+      <style:text-properties fo:color="#ff0000"/>
+      <number:text>(</number:text>
+      <number:currency-symbol/>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text>)</number:text>
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N139P0"/>
+    </number:currency-style>
+    <number:time-style style:name="N140">
+      <number:minutes number:style="long"/>
+      <number:text>:</number:text>
+      <number:seconds number:style="long" number:decimal-places="1"/>
+    </number:time-style>
+    <number:date-style style:name="N141">
+      <number:month/>
+      <number:text>/</number:text>
       <number:day/>
-      <number:text>-</number:text>
-      <number:month number:textual="true"/>
+      <number:text>/</number:text>
+      <number:year number:style="long"/>
     </number:date-style>
-    <number:date-style style:name="N152">
+    <number:date-style style:name="N143">
       <number:day/>
       <number:text>-</number:text>
       <number:month number:textual="true"/>
       <number:text>-</number:text>
       <number:year/>
     </number:date-style>
-    <number:date-style style:name="N151">
-      <number:month/>
-      <number:text>/</number:text>
-      <number:day/>
-      <number:text>/</number:text>
-      <number:year number:style="long"/>
-    </number:date-style>
-    <number:currency-style style:name="N150P0" style:volatile="true">
-      <number:currency-symbol/>
-      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:currency-style>
-    <number:currency-style style:name="N150">
-      <style:text-properties fo:color="#ff0000"/>
-      <number:text>(</number:text>
-      <number:currency-symbol/>
-      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text>)</number:text>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N150P0"/>
-    </number:currency-style>
-    <number:currency-style style:name="N149P0" style:volatile="true">
-      <number:currency-symbol/>
-      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:currency-style>
-    <number:currency-style style:name="N149">
-      <number:text>(</number:text>
-      <number:currency-symbol/>
-      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text>)</number:text>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N149P0"/>
-    </number:currency-style>
-    <number:currency-style style:name="N147P0" style:volatile="true">
-      <number:currency-symbol/>
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:currency-style>
-    <number:currency-style style:name="N147">
-      <style:text-properties fo:color="#ff0000"/>
-      <number:text>(</number:text>
-      <number:currency-symbol/>
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text>)</number:text>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N147P0"/>
-    </number:currency-style>
-    <number:currency-style style:name="N146P0" style:volatile="true">
-      <number:currency-symbol/>
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:currency-style>
-    <number:currency-style style:name="N146">
-      <number:text>(</number:text>
-      <number:currency-symbol/>
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text>)</number:text>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N146P0"/>
-    </number:currency-style>
-    <number:number-style style:name="N144P0" style:volatile="true">
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:number-style>
-    <number:number-style style:name="N144">
-      <style:text-properties fo:color="#ff0000"/>
-      <number:text>(</number:text>
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text>)</number:text>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N144P0"/>
-    </number:number-style>
-    <number:number-style style:name="N142P0" style:volatile="true">
-      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:number-style>
-    <number:number-style style:name="N142">
-      <style:text-properties fo:color="#ff0000"/>
-      <number:text>(</number:text>
-      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text>)</number:text>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N142P0"/>
-    </number:number-style>
-    <number:number-style style:name="N140P0" style:volatile="true">
-      <number:text> </number:text>
-      <number:fill-character> </number:fill-character>
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:number-style>
-    <number:number-style style:name="N140P1" style:volatile="true">
-      <number:text> </number:text>
-      <number:fill-character> </number:fill-character>
-      <number:text>(</number:text>
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text>)</number:text>
-    </number:number-style>
-    <number:number-style style:name="N140P2" style:volatile="true">
-      <number:text> </number:text>
-      <number:fill-character> </number:fill-character>
-      <number:text>- </number:text>
-    </number:number-style>
-    <number:text-style style:name="N140">
-      <number:text> </number:text>
-      <number:text-content/>
-      <number:text> </number:text>
-      <style:map style:condition="value()&gt;0" style:apply-style-name="N140P0"/>
-      <style:map style:condition="value()&lt;0" style:apply-style-name="N140P1"/>
-      <style:map style:condition="value()=0" style:apply-style-name="N140P2"/>
-    </number:text-style>
-    <number:currency-style style:name="N136P0" style:volatile="true">
-      <number:currency-symbol/>
-      <number:fill-character> </number:fill-character>
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:currency-style>
-    <number:currency-style style:name="N136P1" style:volatile="true">
-      <number:currency-symbol/>
-      <number:fill-character> </number:fill-character>
-      <number:text>(</number:text>
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text>)</number:text>
-    </number:currency-style>
-    <number:currency-style style:name="N136P2" style:volatile="true">
-      <number:currency-symbol/>
-      <number:fill-character> </number:fill-character>
-      <number:text>- </number:text>
-    </number:currency-style>
-    <number:text-style style:name="N136">
-      <number:text> </number:text>
-      <number:text-content/>
-      <number:text> </number:text>
-      <style:map style:condition="value()&gt;0" style:apply-style-name="N136P0"/>
-      <style:map style:condition="value()&lt;0" style:apply-style-name="N136P1"/>
-      <style:map style:condition="value()=0" style:apply-style-name="N136P2"/>
-    </number:text-style>
-    <number:number-style style:name="N132P0" style:volatile="true">
-      <number:text> </number:text>
-      <number:fill-character> </number:fill-character>
-      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:number-style>
-    <number:number-style style:name="N132P1" style:volatile="true">
-      <number:text> </number:text>
-      <number:fill-character> </number:fill-character>
-      <number:text>(</number:text>
-      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text>)</number:text>
-    </number:number-style>
-    <number:number-style style:name="N132P2" style:volatile="true">
-      <number:text> </number:text>
-      <number:fill-character> </number:fill-character>
-      <number:text>-</number:text>
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="0"/>
-      <number:text> </number:text>
-    </number:number-style>
-    <number:text-style style:name="N132">
-      <number:text> </number:text>
-      <number:text-content/>
-      <number:text> </number:text>
-      <style:map style:condition="value()&gt;0" style:apply-style-name="N132P0"/>
-      <style:map style:condition="value()&lt;0" style:apply-style-name="N132P1"/>
-      <style:map style:condition="value()=0" style:apply-style-name="N132P2"/>
-    </number:text-style>
-    <number:currency-style style:name="N128P0" style:volatile="true">
-      <number:currency-symbol/>
-      <number:fill-character> </number:fill-character>
-      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:currency-style>
-    <number:currency-style style:name="N128P1" style:volatile="true">
-      <number:currency-symbol/>
-      <number:fill-character> </number:fill-character>
-      <number:text>(</number:text>
-      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text>)</number:text>
-    </number:currency-style>
-    <number:currency-style style:name="N128P2" style:volatile="true">
-      <number:currency-symbol/>
-      <number:fill-character> </number:fill-character>
-      <number:text>-</number:text>
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="0"/>
-      <number:text> </number:text>
-    </number:currency-style>
-    <number:text-style style:name="N128">
-      <number:text> </number:text>
-      <number:text-content/>
-      <number:text> </number:text>
-      <style:map style:condition="value()&gt;0" style:apply-style-name="N128P0"/>
-      <style:map style:condition="value()&lt;0" style:apply-style-name="N128P1"/>
-      <style:map style:condition="value()=0" style:apply-style-name="N128P2"/>
-    </number:text-style>
-    <number:time-style style:name="N124">
-      <number:minutes number:style="long"/>
-      <number:text>:</number:text>
-      <number:seconds number:style="long"/>
-    </number:time-style>
-    <number:time-style style:name="N123" number:truncate-on-overflow="false">
-      <number:hours/>
-      <number:text>:</number:text>
-      <number:minutes number:style="long"/>
-      <number:text>:</number:text>
-      <number:seconds number:style="long"/>
-    </number:time-style>
-    <number:time-style style:name="N122">
-      <number:minutes number:style="long"/>
-      <number:text>:</number:text>
-      <number:seconds number:style="long" number:decimal-places="1"/>
-    </number:time-style>
-    <number:number-style style:name="N121">
-      <number:scientific-number number:decimal-places="1" number:min-decimal-places="1" number:min-integer-digits="1" number:min-exponent-digits="1" number:exponent-interval="3" number:forced-exponent-sign="true"/>
-    </number:number-style>
     <style:style style:name="Default" style:family="table-cell">
       <style:table-cell-properties style:rotation-align="none" style:vertical-align="bottom"/>
       <style:text-properties fo:color="#000000" style:font-name="Calibri" fo:font-family="Calibri" style:font-family-generic="swiss" fo:font-size="11pt" style:font-size-asian="11pt" style:font-name-complex="Calibri" style:font-family-complex="Calibri" style:font-family-generic-complex="swiss" style:font-size-complex="11pt"/>

</xml_diff>

<commit_message>
Improve transaction input UI and balance calculation for early-month entries
- Enhanced add_transaction() with:
  - Time and amount validation using regex
  - Flexible date/time parsing (supports multiple formats)
  - Error messages for invalid input
- Improved display formatting in create_table() (MM-DD-YYYY & 12-hour time)
- Added logic in recalculate_balances() to handle new transactions inserted at the start of the list:
  - If inserted at index 0, reverse-calculates initial balance using the next transaction
  - Ensures consistent balance recalculation moving forward
- Refactored tree/table refresh logic to keep GUI in sync after new entries
-Changed data type in transactions_class_creator to sort data easier
</commit_message>
<xml_diff>
--- a/master_transaction.xlsx
+++ b/master_transaction.xlsx
@@ -65,13 +65,6 @@
       <number:text>/</number:text>
       <number:year/>
     </number:date-style>
-    <number:date-style style:name="N37" number:automatic-order="true">
-      <number:month number:style="long"/>
-      <number:text>/</number:text>
-      <number:day number:style="long"/>
-      <number:text>/</number:text>
-      <number:year/>
-    </number:date-style>
     <number:time-style style:name="N61">
       <number:hours number:style="long"/>
       <number:text>:</number:text>
@@ -79,11 +72,6 @@
       <number:text>:</number:text>
       <number:seconds number:style="long"/>
     </number:time-style>
-    <style:style style:name="ce2" style:family="table-cell" style:parent-style-name="Default">
-      <style:table-cell-properties style:diagonal-bl-tr="none" style:diagonal-tl-br="none" style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="no-wrap" fo:border="0.74pt solid #000000" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="top" loext:vertical-justify="auto"/>
-      <style:paragraph-properties fo:text-align="center" css3t:text-justify="auto" fo:margin-left="0in" style:writing-mode="page"/>
-      <style:text-properties fo:color="#000000" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Calibri" fo:font-size="11pt" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="bold" style:font-size-asian="11pt" style:font-style-asian="normal" style:font-weight-asian="bold" style:font-name-complex="Calibri" style:font-size-complex="11pt" style:font-style-complex="normal" style:font-weight-complex="bold"/>
-    </style:style>
     <style:style style:name="ce3" style:family="table-cell" style:parent-style-name="Default">
       <style:table-cell-properties style:diagonal-bl-tr="none" style:diagonal-tl-br="none" style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="no-wrap" fo:border="0.74pt solid #000000" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="top" loext:vertical-justify="auto"/>
       <style:paragraph-properties fo:text-align="center" css3t:text-justify="auto" fo:margin-left="0in" style:writing-mode="page"/>
@@ -92,7 +80,7 @@
     <style:style style:name="ce5" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N30">
       <style:table-cell-properties style:rotation-align="none"/>
     </style:style>
-    <style:style style:name="ce6" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N37"/>
+    <style:style style:name="ce4" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N30"/>
     <style:style style:name="ce7" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N61"/>
   </office:automatic-styles>
   <office:body>
@@ -174,7 +162,7 @@
           <table:table-cell table:style-name="ce5" office:value-type="date" office:date-value="2025-01-05" calcext:value-type="date">
             <text:p>1/5/25</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce7" office:value-type="string" calcext:value-type="string">
             <text:p>03:28:00</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -192,7 +180,7 @@
           <table:table-cell table:style-name="ce5" office:value-type="date" office:date-value="2025-01-07" calcext:value-type="date">
             <text:p>1/7/25</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce7" office:value-type="string" calcext:value-type="string">
             <text:p>00:06:00</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -210,7 +198,7 @@
           <table:table-cell table:style-name="ce5" office:value-type="date" office:date-value="2025-01-10" calcext:value-type="date">
             <text:p>1/10/25</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce7" office:value-type="string" calcext:value-type="string">
             <text:p>10:16:00</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -228,7 +216,7 @@
           <table:table-cell table:style-name="ce5" office:value-type="date" office:date-value="2025-01-14" calcext:value-type="date">
             <text:p>1/14/25</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce7" office:value-type="string" calcext:value-type="string">
             <text:p>08:08:00</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -246,7 +234,7 @@
           <table:table-cell table:style-name="ce5" office:value-type="date" office:date-value="2025-01-16" calcext:value-type="date">
             <text:p>1/16/25</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce7" office:value-type="string" calcext:value-type="string">
             <text:p>13:09:00</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -264,7 +252,7 @@
           <table:table-cell table:style-name="ce5" office:value-type="date" office:date-value="2025-01-17" calcext:value-type="date">
             <text:p>1/17/25</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce7" office:value-type="string" calcext:value-type="string">
             <text:p>13:20:00</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -282,7 +270,7 @@
           <table:table-cell table:style-name="ce5" office:value-type="date" office:date-value="2025-01-19" calcext:value-type="date">
             <text:p>1/19/25</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce7" office:value-type="string" calcext:value-type="string">
             <text:p>00:44:00</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -300,7 +288,7 @@
           <table:table-cell table:style-name="ce5" office:value-type="date" office:date-value="2025-01-22" calcext:value-type="date">
             <text:p>1/22/25</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce7" office:value-type="string" calcext:value-type="string">
             <text:p>10:11:00</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -318,7 +306,7 @@
           <table:table-cell table:style-name="ce5" office:value-type="date" office:date-value="2025-01-26" calcext:value-type="date">
             <text:p>1/26/25</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce7" office:value-type="string" calcext:value-type="string">
             <text:p>01:01:00</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -336,7 +324,7 @@
           <table:table-cell table:style-name="ce5" office:value-type="date" office:date-value="2025-01-27" calcext:value-type="date">
             <text:p>1/27/25</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce7" office:value-type="string" calcext:value-type="string">
             <text:p>03:37:00</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -354,7 +342,7 @@
           <table:table-cell table:style-name="ce5" office:value-type="date" office:date-value="2025-01-28" calcext:value-type="date">
             <text:p>1/28/25</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce7" office:value-type="string" calcext:value-type="string">
             <text:p>12:15:00</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -372,7 +360,7 @@
           <table:table-cell table:style-name="ce5" office:value-type="date" office:date-value="2025-01-30" calcext:value-type="date">
             <text:p>1/30/25</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce7" office:value-type="string" calcext:value-type="string">
             <text:p>02:04:00</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -390,7 +378,7 @@
           <table:table-cell table:style-name="ce5" office:value-type="date" office:date-value="2025-02-01" calcext:value-type="date">
             <text:p>2/1/25</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce7" office:value-type="string" calcext:value-type="string">
             <text:p>22:05:00</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -408,7 +396,7 @@
           <table:table-cell table:style-name="ce5" office:value-type="date" office:date-value="2025-02-05" calcext:value-type="date">
             <text:p>2/5/25</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce7" office:value-type="string" calcext:value-type="string">
             <text:p>04:48:00</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -426,7 +414,7 @@
           <table:table-cell table:style-name="ce5" office:value-type="date" office:date-value="2025-02-08" calcext:value-type="date">
             <text:p>2/8/25</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce7" office:value-type="string" calcext:value-type="string">
             <text:p>07:01:00</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -444,7 +432,7 @@
           <table:table-cell table:style-name="ce5" office:value-type="date" office:date-value="2025-02-10" calcext:value-type="date">
             <text:p>2/10/25</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce7" office:value-type="string" calcext:value-type="string">
             <text:p>14:04:00</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -462,7 +450,7 @@
           <table:table-cell table:style-name="ce5" office:value-type="date" office:date-value="2025-02-13" calcext:value-type="date">
             <text:p>2/13/25</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce7" office:value-type="string" calcext:value-type="string">
             <text:p>11:45:00</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -480,7 +468,7 @@
           <table:table-cell table:style-name="ce5" office:value-type="date" office:date-value="2025-02-15" calcext:value-type="date">
             <text:p>2/15/25</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce7" office:value-type="string" calcext:value-type="string">
             <text:p>05:10:00</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -498,7 +486,7 @@
           <table:table-cell table:style-name="ce5" office:value-type="date" office:date-value="2025-02-17" calcext:value-type="date">
             <text:p>2/17/25</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce7" office:value-type="string" calcext:value-type="string">
             <text:p>08:23:00</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -516,7 +504,7 @@
           <table:table-cell table:style-name="ce5" office:value-type="date" office:date-value="2025-02-20" calcext:value-type="date">
             <text:p>2/20/25</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce7" office:value-type="string" calcext:value-type="string">
             <text:p>15:36:00</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -531,11 +519,11 @@
           <table:table-cell table:number-columns-repeated="1019"/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
-          <table:table-cell table:style-name="ce6" office:value-type="date" office:date-value="2025-06-05" calcext:value-type="date">
-            <text:p>06/05/25</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce7" office:value-type="time" office:time-value="PT12H25M00S" calcext:value-type="time">
-            <text:p>12:25:00</text:p>
+          <table:table-cell table:style-name="ce4" office:value-type="date" office:date-value="2025-06-05" calcext:value-type="date">
+            <text:p>6/5/25</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce7" office:value-type="string" calcext:value-type="string">
+            <text:p>08:23:00</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Test 21</text:p>
@@ -565,10 +553,10 @@
 <office:document-meta xmlns:grddl="http://www.w3.org/2003/g/data-view#" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:ooo="http://openoffice.org/2004/office" xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" office:version="1.3">
   <office:meta>
     <meta:creation-date>2025-05-26T13:39:43</meta:creation-date>
-    <dc:date>2025-06-08T12:55:16.964991491</dc:date>
+    <dc:date>2025-06-10T20:42:26.632042623</dc:date>
     <meta:generator>LibreOffice/7.3.7.2$Linux_X86_64 LibreOffice_project/30$Build-2</meta:generator>
-    <meta:editing-duration>PT31M7S</meta:editing-duration>
-    <meta:editing-cycles>4</meta:editing-cycles>
+    <meta:editing-duration>PT2H21M52S</meta:editing-duration>
+    <meta:editing-cycles>6</meta:editing-cycles>
     <meta:document-statistic meta:table-count="2" meta:cell-count="118" meta:object-count="0"/>
     <meta:user-defined meta:name="AppVersion">12.0000</meta:user-defined>
   </office:meta>
@@ -602,10 +590,10 @@
               <config:config-item config:name="AnchoredTextOverflowLegacy" config:type="boolean">false</config:config-item>
             </config:config-item-map-entry>
             <config:config-item-map-entry config:name="Transactions">
-              <config:config-item config:name="CursorPositionX" config:type="int">4</config:config-item>
-              <config:config-item config:name="CursorPositionY" config:type="int">22</config:config-item>
+              <config:config-item config:name="CursorPositionX" config:type="int">1</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">31</config:config-item>
               <config:config-item config:name="ActiveSplitRange" config:type="short">2</config:config-item>
-              <config:config-item config:name="PositionLeft" config:type="int">1</config:config-item>
+              <config:config-item config:name="PositionLeft" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionRight" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionTop" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionBottom" config:type="int">0</config:config-item>
@@ -664,7 +652,7 @@
       <config:config-item config:name="LoadReadonly" config:type="boolean">false</config:config-item>
       <config:config-item config:name="PrinterName" config:type="string">Generic Printer</config:config-item>
       <config:config-item config:name="PrinterPaperFromSetup" config:type="boolean">false</config:config-item>
-      <config:config-item config:name="PrinterSetup" config:type="base64Binary">pAH+/0dlbmVyaWMgUHJpbnRlcgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAU0dFTlBSVAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAWAAMAxQAAAAAAAAAIAFZUAAAkbQAASm9iRGF0YSAxCnByaW50ZXI9R2VuZXJpYyBQcmludGVyCm9yaWVudGF0aW9uPVBvcnRyYWl0CmNvcGllcz0xCmNvbGxhdGU9ZmFsc2UKbWFyZ2luYWRqdXN0bWVudD0wLDAsMCwwCmNvbG9yZGVwdGg9MjQKcHNsZXZlbD0wCnBkZmRldmljZT0xCmNvbG9yZGV2aWNlPTAKUFBEQ29udGV4dERhdGEKUGFnZVNpemU6TGV0dGVyAER1cGxleDpOb25lAAASAENPTVBBVF9EVVBMRVhfTU9ERQ8ARHVwbGV4TW9kZTo6T2Zm</config:config-item>
+      <config:config-item config:name="PrinterSetup" config:type="base64Binary">pAH+/0dlbmVyaWMgUHJpbnRlcgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAU0dFTlBSVAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAWAAMAxQAAAAAAAAAIAFZUAAAkbQAASm9iRGF0YSAxCnByaW50ZXI9R2VuZXJpYyBQcmludGVyCm9yaWVudGF0aW9uPVBvcnRyYWl0CmNvcGllcz0xCmNvbGxhdGU9ZmFsc2UKbWFyZ2luYWRqdXN0bWVudD0wLDAsMCwwCmNvbG9yZGVwdGg9MjQKcHNsZXZlbD0wCnBkZmRldmljZT0xCmNvbG9yZGV2aWNlPTAKUFBEQ29udGV4dERhdGEKRHVwbGV4Ok5vbmUAUGFnZVNpemU6TGV0dGVyAAASAENPTVBBVF9EVVBMRVhfTU9ERQ8ARHVwbGV4TW9kZTo6T2Zm</config:config-item>
       <config:config-item config:name="RasterIsVisible" config:type="boolean">false</config:config-item>
       <config:config-item config:name="RasterResolutionX" config:type="int">1270</config:config-item>
       <config:config-item config:name="RasterResolutionY" config:type="int">1270</config:config-item>
@@ -708,267 +696,267 @@
       <number:number number:min-integer-digits="1"/>
     </number:number-style>
     <number:date-style style:name="N159">
-      <number:month/>
-      <number:text>/</number:text>
-      <number:day/>
-      <number:text>/</number:text>
-      <number:year number:style="long"/>
-      <number:text> </number:text>
-      <number:hours/>
-      <number:text>:</number:text>
-      <number:minutes number:style="long"/>
-    </number:date-style>
-    <number:number-style style:name="N157P0" style:volatile="true">
-      <number:text> </number:text>
-      <number:fill-character> </number:fill-character>
-      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:number-style>
-    <number:number-style style:name="N157P1" style:volatile="true">
-      <number:text> </number:text>
-      <number:fill-character> </number:fill-character>
-      <number:text>(</number:text>
-      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text>)</number:text>
-    </number:number-style>
-    <number:number-style style:name="N157P2" style:volatile="true">
-      <number:text> </number:text>
-      <number:fill-character> </number:fill-character>
-      <number:text>-</number:text>
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="0"/>
-      <number:text> </number:text>
-    </number:number-style>
-    <number:text-style style:name="N157">
-      <number:text> </number:text>
-      <number:text-content/>
-      <number:text> </number:text>
-      <style:map style:condition="value()&gt;0" style:apply-style-name="N157P0"/>
-      <style:map style:condition="value()&lt;0" style:apply-style-name="N157P1"/>
-      <style:map style:condition="value()=0" style:apply-style-name="N157P2"/>
-    </number:text-style>
-    <number:time-style style:name="N153">
-      <number:hours/>
-      <number:text>:</number:text>
-      <number:minutes number:style="long"/>
-    </number:time-style>
-    <number:time-style style:name="N152">
-      <number:hours/>
-      <number:text>:</number:text>
-      <number:minutes number:style="long"/>
-      <number:text>:</number:text>
-      <number:seconds number:style="long"/>
-      <number:text> </number:text>
-      <number:am-pm/>
-    </number:time-style>
-    <number:time-style style:name="N151">
-      <number:hours/>
-      <number:text>:</number:text>
-      <number:minutes number:style="long"/>
-      <number:text> </number:text>
-      <number:am-pm/>
-    </number:time-style>
-    <number:currency-style style:name="N149P0" style:volatile="true">
-      <number:currency-symbol/>
-      <number:fill-character> </number:fill-character>
-      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:currency-style>
-    <number:currency-style style:name="N149P1" style:volatile="true">
-      <number:currency-symbol/>
-      <number:fill-character> </number:fill-character>
-      <number:text>(</number:text>
-      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text>)</number:text>
-    </number:currency-style>
-    <number:currency-style style:name="N149P2" style:volatile="true">
-      <number:currency-symbol/>
-      <number:fill-character> </number:fill-character>
-      <number:text>-</number:text>
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="0"/>
-      <number:text> </number:text>
-    </number:currency-style>
-    <number:text-style style:name="N149">
-      <number:text> </number:text>
-      <number:text-content/>
-      <number:text> </number:text>
-      <style:map style:condition="value()&gt;0" style:apply-style-name="N149P0"/>
-      <style:map style:condition="value()&lt;0" style:apply-style-name="N149P1"/>
-      <style:map style:condition="value()=0" style:apply-style-name="N149P2"/>
-    </number:text-style>
-    <number:date-style style:name="N145">
       <number:day/>
       <number:text>-</number:text>
-      <number:month number:textual="true"/>
-    </number:date-style>
-    <number:time-style style:name="N144">
-      <number:minutes number:style="long"/>
-      <number:text>:</number:text>
-      <number:seconds number:style="long"/>
-    </number:time-style>
-    <number:date-style style:name="N150">
       <number:month number:textual="true"/>
       <number:text>-</number:text>
       <number:year/>
     </number:date-style>
-    <number:number-style style:name="N121">
-      <number:scientific-number number:decimal-places="1" number:min-decimal-places="1" number:min-integer-digits="1" number:min-exponent-digits="1" number:exponent-interval="3" number:forced-exponent-sign="true"/>
-    </number:number-style>
-    <number:currency-style style:name="N125P0" style:volatile="true">
-      <number:currency-symbol/>
-      <number:fill-character> </number:fill-character>
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:currency-style>
-    <number:currency-style style:name="N125P1" style:volatile="true">
-      <number:currency-symbol/>
-      <number:fill-character> </number:fill-character>
-      <number:text>(</number:text>
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text>)</number:text>
-    </number:currency-style>
-    <number:currency-style style:name="N125P2" style:volatile="true">
-      <number:currency-symbol/>
-      <number:fill-character> </number:fill-character>
-      <number:text>- </number:text>
-    </number:currency-style>
-    <number:text-style style:name="N125">
-      <number:text> </number:text>
-      <number:text-content/>
-      <number:text> </number:text>
-      <style:map style:condition="value()&gt;0" style:apply-style-name="N125P0"/>
-      <style:map style:condition="value()&lt;0" style:apply-style-name="N125P1"/>
-      <style:map style:condition="value()=0" style:apply-style-name="N125P2"/>
-    </number:text-style>
-    <number:currency-style style:name="N138P0" style:volatile="true">
-      <number:currency-symbol/>
-      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:currency-style>
-    <number:currency-style style:name="N138">
-      <number:text>(</number:text>
-      <number:currency-symbol/>
-      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text>)</number:text>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N138P0"/>
-    </number:currency-style>
-    <number:time-style style:name="N158">
-      <number:hours/>
-      <number:text>:</number:text>
-      <number:minutes number:style="long"/>
-      <number:text>:</number:text>
-      <number:seconds number:style="long"/>
-    </number:time-style>
-    <number:number-style style:name="N129P0" style:volatile="true">
-      <number:text> </number:text>
-      <number:fill-character> </number:fill-character>
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:number-style>
-    <number:number-style style:name="N129P1" style:volatile="true">
-      <number:text> </number:text>
-      <number:fill-character> </number:fill-character>
-      <number:text>(</number:text>
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text>)</number:text>
-    </number:number-style>
-    <number:number-style style:name="N129P2" style:volatile="true">
-      <number:text> </number:text>
-      <number:fill-character> </number:fill-character>
-      <number:text>- </number:text>
-    </number:number-style>
-    <number:text-style style:name="N129">
-      <number:text> </number:text>
-      <number:text-content/>
-      <number:text> </number:text>
-      <style:map style:condition="value()&gt;0" style:apply-style-name="N129P0"/>
-      <style:map style:condition="value()&lt;0" style:apply-style-name="N129P1"/>
-      <style:map style:condition="value()=0" style:apply-style-name="N129P2"/>
-    </number:text-style>
-    <number:time-style style:name="N142" number:truncate-on-overflow="false">
-      <number:hours/>
-      <number:text>:</number:text>
-      <number:minutes number:style="long"/>
-      <number:text>:</number:text>
-      <number:seconds number:style="long"/>
-    </number:time-style>
-    <number:number-style style:name="N131P0" style:volatile="true">
-      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:number-style>
-    <number:number-style style:name="N131">
-      <style:text-properties fo:color="#ff0000"/>
-      <number:text>(</number:text>
-      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text>)</number:text>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N131P0"/>
-    </number:number-style>
-    <number:number-style style:name="N133P0" style:volatile="true">
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:number-style>
-    <number:number-style style:name="N133">
-      <style:text-properties fo:color="#ff0000"/>
-      <number:text>(</number:text>
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text>)</number:text>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N133P0"/>
-    </number:number-style>
-    <number:currency-style style:name="N135P0" style:volatile="true">
-      <number:currency-symbol/>
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:currency-style>
-    <number:currency-style style:name="N135">
-      <number:text>(</number:text>
-      <number:currency-symbol/>
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text>)</number:text>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N135P0"/>
-    </number:currency-style>
-    <number:currency-style style:name="N136P0" style:volatile="true">
-      <number:currency-symbol/>
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:currency-style>
-    <number:currency-style style:name="N136">
-      <style:text-properties fo:color="#ff0000"/>
-      <number:text>(</number:text>
-      <number:currency-symbol/>
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text>)</number:text>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N136P0"/>
-    </number:currency-style>
-    <number:currency-style style:name="N139P0" style:volatile="true">
-      <number:currency-symbol/>
-      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:currency-style>
-    <number:currency-style style:name="N139">
-      <style:text-properties fo:color="#ff0000"/>
-      <number:text>(</number:text>
-      <number:currency-symbol/>
-      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text>)</number:text>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N139P0"/>
-    </number:currency-style>
-    <number:time-style style:name="N140">
-      <number:minutes number:style="long"/>
-      <number:text>:</number:text>
-      <number:seconds number:style="long" number:decimal-places="1"/>
-    </number:time-style>
-    <number:date-style style:name="N141">
+    <number:date-style style:name="N158">
       <number:month/>
       <number:text>/</number:text>
       <number:day/>
       <number:text>/</number:text>
       <number:year number:style="long"/>
     </number:date-style>
-    <number:date-style style:name="N143">
+    <number:time-style style:name="N157">
+      <number:minutes number:style="long"/>
+      <number:text>:</number:text>
+      <number:seconds number:style="long" number:decimal-places="1"/>
+    </number:time-style>
+    <number:currency-style style:name="N156P0" style:volatile="true">
+      <number:currency-symbol/>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:currency-style>
+    <number:currency-style style:name="N156">
+      <style:text-properties fo:color="#ff0000"/>
+      <number:text>(</number:text>
+      <number:currency-symbol/>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text>)</number:text>
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N156P0"/>
+    </number:currency-style>
+    <number:currency-style style:name="N155P0" style:volatile="true">
+      <number:currency-symbol/>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:currency-style>
+    <number:currency-style style:name="N155">
+      <style:text-properties fo:color="#ff0000"/>
+      <number:text>(</number:text>
+      <number:currency-symbol/>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text>)</number:text>
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N155P0"/>
+    </number:currency-style>
+    <number:currency-style style:name="N154P0" style:volatile="true">
+      <number:currency-symbol/>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:currency-style>
+    <number:currency-style style:name="N154">
+      <number:text>(</number:text>
+      <number:currency-symbol/>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text>)</number:text>
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N154P0"/>
+    </number:currency-style>
+    <number:number-style style:name="N152P0" style:volatile="true">
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:number-style>
+    <number:number-style style:name="N152">
+      <style:text-properties fo:color="#ff0000"/>
+      <number:text>(</number:text>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text>)</number:text>
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N152P0"/>
+    </number:number-style>
+    <number:number-style style:name="N150P0" style:volatile="true">
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:number-style>
+    <number:number-style style:name="N150">
+      <style:text-properties fo:color="#ff0000"/>
+      <number:text>(</number:text>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text>)</number:text>
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N150P0"/>
+    </number:number-style>
+    <number:time-style style:name="N148" number:truncate-on-overflow="false">
+      <number:hours/>
+      <number:text>:</number:text>
+      <number:minutes number:style="long"/>
+      <number:text>:</number:text>
+      <number:seconds number:style="long"/>
+    </number:time-style>
+    <number:number-style style:name="N147P0" style:volatile="true">
+      <number:text> </number:text>
+      <number:fill-character> </number:fill-character>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:number-style>
+    <number:number-style style:name="N147P1" style:volatile="true">
+      <number:text> </number:text>
+      <number:fill-character> </number:fill-character>
+      <number:text>(</number:text>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text>)</number:text>
+    </number:number-style>
+    <number:number-style style:name="N147P2" style:volatile="true">
+      <number:text> </number:text>
+      <number:fill-character> </number:fill-character>
+      <number:text>- </number:text>
+    </number:number-style>
+    <number:text-style style:name="N147">
+      <number:text> </number:text>
+      <number:text-content/>
+      <number:text> </number:text>
+      <style:map style:condition="value()&gt;0" style:apply-style-name="N147P0"/>
+      <style:map style:condition="value()&lt;0" style:apply-style-name="N147P1"/>
+      <style:map style:condition="value()=0" style:apply-style-name="N147P2"/>
+    </number:text-style>
+    <number:time-style style:name="N143">
+      <number:hours/>
+      <number:text>:</number:text>
+      <number:minutes number:style="long"/>
+      <number:text>:</number:text>
+      <number:seconds number:style="long"/>
+    </number:time-style>
+    <number:currency-style style:name="N142P0" style:volatile="true">
+      <number:currency-symbol/>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:currency-style>
+    <number:currency-style style:name="N142">
+      <number:text>(</number:text>
+      <number:currency-symbol/>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text>)</number:text>
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N142P0"/>
+    </number:currency-style>
+    <number:currency-style style:name="N140P0" style:volatile="true">
+      <number:currency-symbol/>
+      <number:fill-character> </number:fill-character>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:currency-style>
+    <number:currency-style style:name="N140P1" style:volatile="true">
+      <number:currency-symbol/>
+      <number:fill-character> </number:fill-character>
+      <number:text>(</number:text>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text>)</number:text>
+    </number:currency-style>
+    <number:currency-style style:name="N140P2" style:volatile="true">
+      <number:currency-symbol/>
+      <number:fill-character> </number:fill-character>
+      <number:text>- </number:text>
+    </number:currency-style>
+    <number:text-style style:name="N140">
+      <number:text> </number:text>
+      <number:text-content/>
+      <number:text> </number:text>
+      <style:map style:condition="value()&gt;0" style:apply-style-name="N140P0"/>
+      <style:map style:condition="value()&lt;0" style:apply-style-name="N140P1"/>
+      <style:map style:condition="value()=0" style:apply-style-name="N140P2"/>
+    </number:text-style>
+    <number:number-style style:name="N136">
+      <number:scientific-number number:decimal-places="1" number:min-decimal-places="1" number:min-integer-digits="1" number:min-exponent-digits="1" number:exponent-interval="3" number:forced-exponent-sign="true"/>
+    </number:number-style>
+    <number:date-style style:name="N135">
+      <number:month number:textual="true"/>
+      <number:text>-</number:text>
+      <number:year/>
+    </number:date-style>
+    <number:time-style style:name="N134">
+      <number:minutes number:style="long"/>
+      <number:text>:</number:text>
+      <number:seconds number:style="long"/>
+    </number:time-style>
+    <number:date-style style:name="N133">
       <number:day/>
       <number:text>-</number:text>
       <number:month number:textual="true"/>
+    </number:date-style>
+    <number:currency-style style:name="N132P0" style:volatile="true">
+      <number:currency-symbol/>
+      <number:fill-character> </number:fill-character>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:currency-style>
+    <number:currency-style style:name="N132P1" style:volatile="true">
+      <number:currency-symbol/>
+      <number:fill-character> </number:fill-character>
+      <number:text>(</number:text>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text>)</number:text>
+    </number:currency-style>
+    <number:currency-style style:name="N132P2" style:volatile="true">
+      <number:currency-symbol/>
+      <number:fill-character> </number:fill-character>
       <number:text>-</number:text>
-      <number:year/>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="0"/>
+      <number:text> </number:text>
+    </number:currency-style>
+    <number:text-style style:name="N132">
+      <number:text> </number:text>
+      <number:text-content/>
+      <number:text> </number:text>
+      <style:map style:condition="value()&gt;0" style:apply-style-name="N132P0"/>
+      <style:map style:condition="value()&lt;0" style:apply-style-name="N132P1"/>
+      <style:map style:condition="value()=0" style:apply-style-name="N132P2"/>
+    </number:text-style>
+    <number:time-style style:name="N128">
+      <number:hours/>
+      <number:text>:</number:text>
+      <number:minutes number:style="long"/>
+      <number:text> </number:text>
+      <number:am-pm/>
+    </number:time-style>
+    <number:time-style style:name="N127">
+      <number:hours/>
+      <number:text>:</number:text>
+      <number:minutes number:style="long"/>
+      <number:text>:</number:text>
+      <number:seconds number:style="long"/>
+      <number:text> </number:text>
+      <number:am-pm/>
+    </number:time-style>
+    <number:time-style style:name="N126">
+      <number:hours/>
+      <number:text>:</number:text>
+      <number:minutes number:style="long"/>
+    </number:time-style>
+    <number:number-style style:name="N125P0" style:volatile="true">
+      <number:text> </number:text>
+      <number:fill-character> </number:fill-character>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:number-style>
+    <number:number-style style:name="N125P1" style:volatile="true">
+      <number:text> </number:text>
+      <number:fill-character> </number:fill-character>
+      <number:text>(</number:text>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text>)</number:text>
+    </number:number-style>
+    <number:number-style style:name="N125P2" style:volatile="true">
+      <number:text> </number:text>
+      <number:fill-character> </number:fill-character>
+      <number:text>-</number:text>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="0"/>
+      <number:text> </number:text>
+    </number:number-style>
+    <number:text-style style:name="N125">
+      <number:text> </number:text>
+      <number:text-content/>
+      <number:text> </number:text>
+      <style:map style:condition="value()&gt;0" style:apply-style-name="N125P0"/>
+      <style:map style:condition="value()&lt;0" style:apply-style-name="N125P1"/>
+      <style:map style:condition="value()=0" style:apply-style-name="N125P2"/>
+    </number:text-style>
+    <number:date-style style:name="N121">
+      <number:month/>
+      <number:text>/</number:text>
+      <number:day/>
+      <number:text>/</number:text>
+      <number:year number:style="long"/>
+      <number:text> </number:text>
+      <number:hours/>
+      <number:text>:</number:text>
+      <number:minutes number:style="long"/>
     </number:date-style>
     <style:style style:name="Default" style:family="table-cell">
       <style:table-cell-properties style:rotation-align="none" style:vertical-align="bottom"/>

</xml_diff>